<commit_message>
add more zoomify images
</commit_message>
<xml_diff>
--- a/docs/15/Template_Oelsande_Kanada_csm.xlsx
+++ b/docs/15/Template_Oelsande_Kanada_csm.xlsx
@@ -940,7 +940,7 @@
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="M/D/YYYY"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1016,12 +1016,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF3333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1092,7 +1086,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1141,10 +1135,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1177,10 +1167,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1189,7 +1175,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Note" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -1268,11 +1254,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9959514170041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1052631578947"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7125506072874"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.9959514170041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1052631578947"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1472,8 +1458,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0283400809717"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
@@ -1515,8 +1501,8 @@
   </sheetPr>
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E44" activeCellId="0" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1524,12 +1510,12 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.0242914979757"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5303643724696"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.4534412955466"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.748987854251"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1650,7 +1636,7 @@
       <c r="I5" s="10" t="n">
         <v>43850</v>
       </c>
-      <c r="L5" s="12"/>
+      <c r="L5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -1671,7 +1657,7 @@
       <c r="I6" s="10" t="n">
         <v>43840</v>
       </c>
-      <c r="L6" s="12"/>
+      <c r="L6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -1732,7 +1718,7 @@
       <c r="I9" s="10" t="n">
         <v>43819</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="L9" s="11" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1795,7 +1781,7 @@
       <c r="I12" s="10" t="n">
         <v>43850</v>
       </c>
-      <c r="L12" s="12"/>
+      <c r="L12" s="11"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -1816,7 +1802,7 @@
       <c r="I13" s="10" t="n">
         <v>43850</v>
       </c>
-      <c r="L13" s="12"/>
+      <c r="L13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
@@ -1837,7 +1823,7 @@
       <c r="I14" s="10" t="n">
         <v>43864</v>
       </c>
-      <c r="L14" s="12"/>
+      <c r="L14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -1860,43 +1846,43 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="12" t="n">
+      <c r="C16" s="11" t="n">
         <v>2012</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="15" t="s">
+      <c r="F16" s="11"/>
+      <c r="G16" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="I16" s="17"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="12" t="s">
         <v>93</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>2020</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>94</v>
       </c>
       <c r="F17" s="0" t="s">
@@ -1910,13 +1896,13 @@
       <c r="A18" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="12" t="n">
+      <c r="C18" s="11" t="n">
         <v>2020</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>97</v>
       </c>
       <c r="F18" s="0" t="s">
@@ -1987,31 +1973,31 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C22" s="12" t="n">
+      <c r="C22" s="11" t="n">
         <v>2016</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="15" t="s">
+      <c r="F22" s="11"/>
+      <c r="G22" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="H22" s="13" t="s">
+      <c r="H22" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="I22" s="17"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
@@ -2037,7 +2023,7 @@
       <c r="A24" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>117</v>
       </c>
       <c r="C24" s="0" t="n">
@@ -2063,13 +2049,13 @@
       <c r="C25" s="0" t="n">
         <v>2017</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="G25" s="20" t="s">
+      <c r="G25" s="19" t="s">
         <v>123</v>
       </c>
       <c r="H25" s="0" t="s">
@@ -2083,13 +2069,13 @@
       <c r="A26" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="C26" s="12" t="n">
+      <c r="C26" s="11" t="n">
         <v>2019</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="12" t="s">
         <v>126</v>
       </c>
       <c r="F26" s="0" t="s">
@@ -2143,22 +2129,22 @@
       <c r="A29" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C29" s="12" t="n">
+      <c r="C29" s="11" t="n">
         <v>2017</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="E29" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="G29" s="20" t="s">
+      <c r="G29" s="19" t="s">
         <v>138</v>
       </c>
       <c r="I29" s="10"/>
@@ -2167,19 +2153,19 @@
       <c r="A30" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="C30" s="12" t="n">
+      <c r="C30" s="11" t="n">
         <v>1981</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="G30" s="20" t="s">
+      <c r="G30" s="19" t="s">
         <v>142</v>
       </c>
       <c r="H30" s="0" t="s">
@@ -2228,29 +2214,29 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="C33" s="12" t="n">
+      <c r="C33" s="11" t="n">
         <v>2016</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="E33" s="18" t="s">
+      <c r="E33" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="13" t="s">
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="K33" s="13" t="s">
+      <c r="K33" s="12" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2298,7 +2284,7 @@
       <c r="A36" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="12" t="s">
         <v>161</v>
       </c>
       <c r="C36" s="0" t="n">
@@ -2335,31 +2321,31 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="C38" s="12" t="n">
+      <c r="C38" s="11" t="n">
         <v>2009</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="E38" s="18" t="s">
+      <c r="E38" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="F38" s="12"/>
-      <c r="G38" s="15" t="s">
+      <c r="F38" s="11"/>
+      <c r="G38" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="H38" s="16" t="s">
+      <c r="H38" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="I38" s="17"/>
-      <c r="J38" s="12"/>
-      <c r="K38" s="12"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
@@ -2382,66 +2368,66 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="C40" s="12" t="n">
+      <c r="C40" s="11" t="n">
         <v>2016</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="E40" s="12"/>
-      <c r="F40" s="13" t="s">
+      <c r="E40" s="11"/>
+      <c r="F40" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="17" t="n">
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="16" t="n">
         <v>43844</v>
       </c>
-      <c r="J40" s="12"/>
-      <c r="K40" s="12"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="C41" s="12" t="n">
+      <c r="C41" s="11" t="n">
         <v>2020</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="E41" s="12"/>
-      <c r="F41" s="13" t="s">
+      <c r="E41" s="11"/>
+      <c r="F41" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="17" t="n">
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="16" t="n">
         <v>43845</v>
       </c>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="C42" s="12" t="n">
+      <c r="C42" s="11" t="n">
         <v>2016</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="12" t="s">
         <v>181</v>
       </c>
       <c r="F42" s="0" t="s">
@@ -2475,16 +2461,16 @@
       <c r="A44" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="15" t="s">
         <v>185</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>2017</v>
       </c>
-      <c r="D44" s="19" t="s">
+      <c r="D44" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="G44" s="20" t="s">
+      <c r="G44" s="19" t="s">
         <v>187</v>
       </c>
       <c r="H44" s="0" t="s">
@@ -2501,10 +2487,10 @@
       <c r="B45" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C45" s="12" t="n">
+      <c r="C45" s="11" t="n">
         <v>2020</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="D45" s="12" t="s">
         <v>190</v>
       </c>
       <c r="F45" s="11" t="s">
@@ -2518,7 +2504,7 @@
       <c r="A46" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="12" t="s">
         <v>192</v>
       </c>
       <c r="C46" s="0" t="n">
@@ -2742,8 +2728,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>

</xml_diff>